<commit_message>
nono commit, 28/10 atualizações
</commit_message>
<xml_diff>
--- a/relatorios/relatorio_carrinhos_11_2025.xlsx
+++ b/relatorios/relatorio_carrinhos_11_2025.xlsx
@@ -16,10 +16,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="yyyy-mm-dd"/>
-    <numFmt numFmtId="165" formatCode="DD/MM/YYYY"/>
-  </numFmts>
+  <numFmts count="0"/>
   <fonts count="5">
     <font>
       <name val="Calibri"/>
@@ -47,11 +44,13 @@
       <sz val="12"/>
     </font>
     <font>
-      <b val="1"/>
-      <color rgb="00000000"/>
+      <name val="Segoe UI"/>
+      <i val="1"/>
+      <color rgb="007F8C8D"/>
+      <sz val="12"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill/>
     </fill>
@@ -68,12 +67,6 @@
       <patternFill patternType="solid">
         <fgColor rgb="0034495E"/>
         <bgColor rgb="0034495E"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="00F1C40F"/>
-        <bgColor rgb="00F1C40F"/>
       </patternFill>
     </fill>
   </fills>
@@ -95,7 +88,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
@@ -106,16 +99,10 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -481,7 +468,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -546,55 +533,20 @@
     <row r="5">
       <c r="A5" s="4" t="inlineStr">
         <is>
-          <t>teste</t>
-        </is>
-      </c>
-      <c r="B5" s="5" t="n">
-        <v>45928</v>
-      </c>
-      <c r="C5" s="5" t="n">
-        <v>45988</v>
-      </c>
-      <c r="D5" s="4" t="n">
-        <v>60</v>
-      </c>
-      <c r="E5" s="6" t="inlineStr">
-        <is>
-          <t>A VENCER</t>
-        </is>
-      </c>
-      <c r="F5" s="7" t="inlineStr">
-        <is>
-          <t>teste</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
-      <c r="A6" s="4" t="inlineStr">
-        <is>
-          <t>teste_periodicidade</t>
-        </is>
-      </c>
-      <c r="B6" s="5" t="n">
-        <v>45929</v>
-      </c>
-      <c r="C6" s="5" t="n">
-        <v>45989</v>
-      </c>
-      <c r="D6" s="4" t="n">
-        <v>60</v>
-      </c>
-      <c r="E6" s="6" t="inlineStr">
-        <is>
-          <t>A VENCER</t>
-        </is>
-      </c>
-      <c r="F6" s="7" t="inlineStr"/>
+          <t>Não há carrinhos para relatar neste período.</t>
+        </is>
+      </c>
+      <c r="B5" s="5" t="n"/>
+      <c r="C5" s="5" t="n"/>
+      <c r="D5" s="5" t="n"/>
+      <c r="E5" s="5" t="n"/>
+      <c r="F5" s="5" t="n"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="3">
     <mergeCell ref="A2:F2"/>
     <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A5:F5"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>